<commit_message>
CBSE Assignment - Done
CBSE Assignment - Done
</commit_message>
<xml_diff>
--- a/CBSE Timelog.xlsx
+++ b/CBSE Timelog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>Task 1</t>
   </si>
@@ -34,6 +34,27 @@
   </si>
   <si>
     <t>Hours:</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>Task2</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>28h</t>
+  </si>
+  <si>
+    <t>Total Assignment time:</t>
+  </si>
+  <si>
+    <t>Total Task time:</t>
+  </si>
+  <si>
+    <t>43h</t>
   </si>
 </sst>
 </file>
@@ -399,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -485,60 +506,255 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>42020</v>
       </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>42021</v>
       </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42022</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42023</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42024</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42025</v>
+      </c>
+      <c r="B44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>42026</v>
+      </c>
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>42027</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>42028</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>42022</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>42029</v>
+      </c>
+      <c r="B62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>42030</v>
+      </c>
+      <c r="B66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>